<commit_message>
update telegram,pip from requirements.txt
</commit_message>
<xml_diff>
--- a/calculator_data.xlsx
+++ b/calculator_data.xlsx
@@ -505,7 +505,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>fcff</t>
+          <t>ff</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -530,7 +530,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -577,13 +577,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
delete /submit from main.py to /
</commit_message>
<xml_diff>
--- a/calculator_data.xlsx
+++ b/calculator_data.xlsx
@@ -505,7 +505,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ddd</t>
+          <t>gg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -530,7 +530,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -555,7 +555,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -598,7 +598,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
change link in index
</commit_message>
<xml_diff>
--- a/calculator_data.xlsx
+++ b/calculator_data.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,7 +505,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>богдана</t>
+          <t>iiandjdmd</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -567,201 +567,77 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>богдана</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Відсутній</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>Підсумок</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>богдана</t>
+          <t>Будуть</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Відсутній</t>
+          <t>Не будуть</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Не знаю</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>Відмітилось</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Підсумок</t>
-        </is>
+      <c r="A5" t="n">
+        <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Будуть</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Не будуть</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Не знаю</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Відмітилось</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change line in index.html
</commit_message>
<xml_diff>
--- a/calculator_data.xlsx
+++ b/calculator_data.xlsx
@@ -503,6 +503,16 @@
       <c r="M1" s="1" t="n"/>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>богдана</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Відсутній</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>0</t>
@@ -561,7 +571,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -621,13 +631,13 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change link to backend
</commit_message>
<xml_diff>
--- a/calculator_data.xlsx
+++ b/calculator_data.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,139 +567,77 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>богдана</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Відсутній</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>Підсумок</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Підсумок</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
+          <t>Будуть</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Не будуть</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Не знаю</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Відмітилось</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Будуть</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Не будуть</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Не знаю</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Відмітилось</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2</v>
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>